<commit_message>
User submitted updates minor edits
</commit_message>
<xml_diff>
--- a/docs/build/html/_downloads/c2b2dd48004b905a08f8647b167b3c1d/damstemplate5272022.xlsx
+++ b/docs/build/html/_downloads/c2b2dd48004b905a08f8647b167b3c1d/damstemplate5272022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CABD\GitHub\Canadian-Wildlife-Federation\Documentation\docs\source\docs_user\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBFACDE-FDC3-42C2-A4D3-E1CECA59809B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A12D08B-C493-4E23-B2DD-6AB5C2F94963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24990" yWindow="2800" windowWidth="20010" windowHeight="14300" xr2:uid="{8510FF68-7378-4877-BC33-372696FC9882}"/>
+    <workbookView xWindow="25340" yWindow="1600" windowWidth="16330" windowHeight="8630" xr2:uid="{8510FF68-7378-4877-BC33-372696FC9882}"/>
   </bookViews>
   <sheets>
     <sheet name="new_data" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="144">
   <si>
     <t>cabd_id</t>
   </si>
@@ -891,7 +891,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -987,9 +987,6 @@
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>141</v>
-      </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
@@ -1894,9 +1891,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2123,27 +2123,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B103F181-233E-4DEC-9ADC-31149E3FC4B0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE4609A-9376-4E3F-8C1A-0281507B16A9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="411171ba-2276-4762-a69b-ae0a1d76a912"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2168,9 +2156,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE4609A-9376-4E3F-8C1A-0281507B16A9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B103F181-233E-4DEC-9ADC-31149E3FC4B0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="411171ba-2276-4762-a69b-ae0a1d76a912"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b7b7ce10-0fd6-45e3-a641-e6fecf0ad4e9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>